<commit_message>
add prediction result xlsx
</commit_message>
<xml_diff>
--- a/chapter2/input/chapter2_demo_data_prediction_result.xlsx
+++ b/chapter2/input/chapter2_demo_data_prediction_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\執筆\practical-mi-guide\chapter2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDF85BE-A031-41D9-BB7C-0C1F9A5AD144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F540D1D6-8509-4565-A99D-03C565D6F19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17800" yWindow="8970" windowWidth="19380" windowHeight="11390" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
+    <workbookView xWindow="17800" yWindow="2560" windowWidth="20390" windowHeight="17850" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="モデル性能一覧" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
   <si>
     <t>画像濃度</t>
     <rPh sb="0" eb="4">
@@ -59,13 +59,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>保存後粘度</t>
-    <rPh sb="0" eb="5">
-      <t>ホゾンゴネンド</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>耐擦過性(n10</t>
     <rPh sb="0" eb="1">
       <t>タイ</t>
@@ -79,17 +72,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>保存後状態</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>DP_test_01</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>DP_test_02</t>
-  </si>
-  <si>
     <t>DP_test_03</t>
   </si>
   <si>
@@ -121,6 +107,315 @@
   </si>
   <si>
     <t>R2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サンプルID</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>高い方が良い
+1-5のランク評価
+5が目標</t>
+    <rPh sb="0" eb="1">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ヒョウカ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>モクヒョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>高い方が良い
+1.4以上が目標</t>
+    <rPh sb="0" eb="1">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ホウ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>モクヒョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>12以下</t>
+    <rPh sb="2" eb="4">
+      <t>イカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>30－38</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>目標</t>
+    <rPh sb="0" eb="2">
+      <t>モクヒョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DP_test_02,DP_033</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>×</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>粘度がDP_033以上のため保存後粘度未達の可能性高い</t>
+    <rPh sb="0" eb="2">
+      <t>ネンド</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="14" eb="19">
+      <t>ホゾンゴネンド</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>ミタツ</t>
+    </rPh>
+    <rPh sb="22" eb="25">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>タカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>予測値に対する評価</t>
+    <rPh sb="0" eb="3">
+      <t>ヨソクチ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>ヒョウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>次回実験への採用優先度</t>
+    <rPh sb="0" eb="4">
+      <t>ジカイジッケン</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>サイヨウ</t>
+    </rPh>
+    <rPh sb="8" eb="11">
+      <t>ユウセンド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>表面張力の値が下限値近辺の可能性がある
+画像濃度は目標値未達の可能性が高い</t>
+    <rPh sb="0" eb="4">
+      <t>ヒョウメンチョウリョク</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>カゲンチ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>キンペン</t>
+    </rPh>
+    <rPh sb="13" eb="16">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="20" eb="24">
+      <t>ガゾウノウド</t>
+    </rPh>
+    <rPh sb="25" eb="28">
+      <t>モクヒョウチ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>ミタツ</t>
+    </rPh>
+    <rPh sb="31" eb="34">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>タカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>目標値を満たす可能性がある</t>
+    <rPh sb="0" eb="3">
+      <t>モクヒョウチ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ミ</t>
+    </rPh>
+    <rPh sb="7" eb="10">
+      <t>カノウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>〇</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画像濃度が予測値から上振れすれば目標値達成の可能性がある
+上振れの程度もRMSEよりも小さい量であり、ある程度可能性は残されていると推察できる</t>
+    <rPh sb="0" eb="4">
+      <t>ガゾウノウド</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>ヨソクチ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ウワブ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>モクヒョウチ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>タッセイ</t>
+    </rPh>
+    <rPh sb="22" eb="25">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>ウワブ</t>
+    </rPh>
+    <rPh sb="33" eb="35">
+      <t>テイド</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>チイ</t>
+    </rPh>
+    <rPh sb="46" eb="47">
+      <t>リョウ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>テイド</t>
+    </rPh>
+    <rPh sb="55" eb="58">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="59" eb="60">
+      <t>ノコ</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>スイサツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画像濃度が予測値から上振れすれば目標値達成の可能性がある
+ただし、RMSEと同じ程度上振れの必要があり、目標値達成の可能性はそこまで高くないと推察できる</t>
+    <rPh sb="0" eb="4">
+      <t>ガゾウノウド</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>ヨソクチ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ウワブ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>モクヒョウチ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>タッセイ</t>
+    </rPh>
+    <rPh sb="22" eb="25">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>テイド</t>
+    </rPh>
+    <rPh sb="42" eb="44">
+      <t>ウワブ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="52" eb="57">
+      <t>モクヒョウチタッセイ</t>
+    </rPh>
+    <rPh sb="58" eb="61">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="66" eb="67">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="71" eb="73">
+      <t>スイサツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>画像濃度が予測値から上振れすれば目標値達成の可能性がある
+ただし、RMSE以上の上振れの必要があり、目標値達成の可能性はそこまで高くないと推察できる</t>
+    <rPh sb="0" eb="4">
+      <t>ガゾウノウド</t>
+    </rPh>
+    <rPh sb="5" eb="8">
+      <t>ヨソクチ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ウワブ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>モクヒョウチ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>タッセイ</t>
+    </rPh>
+    <rPh sb="22" eb="25">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>ウワブ</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="50" eb="55">
+      <t>モクヒョウチタッセイ</t>
+    </rPh>
+    <rPh sb="56" eb="59">
+      <t>カノウセイ</t>
+    </rPh>
+    <rPh sb="64" eb="65">
+      <t>タカ</t>
+    </rPh>
+    <rPh sb="69" eb="71">
+      <t>スイサツ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -128,7 +423,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="184" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -141,15 +439,6 @@
       <sz val="6"/>
       <name val="游ゴシック"/>
       <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -170,7 +459,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -193,30 +482,307 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="184" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="184" formatCode="0.0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -227,6 +793,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00609110-2842-4AC5-9FD3-A1A8B4FDA806}" name="テーブル1" displayName="テーブル1" ref="D11:J20" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
+  <autoFilter ref="D11:J20" xr:uid="{00609110-2842-4AC5-9FD3-A1A8B4FDA806}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{85CEFAB7-CA72-47D8-8B13-90460514BFEC}" name="サンプルID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{6230F9C7-6651-4570-8383-C3596721A59D}" name="耐擦過性(n10" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B9657BD6-C716-4D0A-B59F-DE7249B4BB67}" name="画像濃度" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{5190B858-94B9-4FFA-AFD0-9DB2E8C9CC11}" name="表面張力" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{CE35112C-631F-497E-BB69-552361CABEF5}" name="粘度" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{0252730B-9FD0-4AB5-9C8C-8D6082BFE834}" name="予測値に対する評価"/>
+    <tableColumn id="9" xr3:uid="{FA0EEA02-82EE-44AD-B464-D28E0666A4F8}" name="次回実験への採用優先度"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,162 +1108,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3433FF01-647B-4F50-A819-EDB9541AAB09}">
-  <dimension ref="D2:J15"/>
+  <dimension ref="D2:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54.5" customWidth="1"/>
+    <col min="10" max="10" width="24.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="4:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="E5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.9</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.23</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="8" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.65</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="E6" s="1" t="s">
+      <c r="E11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+      <c r="D12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7">
+      <c r="E12" s="10">
+        <v>5.1500635499999996</v>
+      </c>
+      <c r="F12" s="8">
         <v>1.51666049</v>
       </c>
-      <c r="G7">
+      <c r="G12" s="12">
+        <v>32.586979229999997</v>
+      </c>
+      <c r="H12" s="8">
         <v>9.5169317800000002</v>
       </c>
-    </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>1.4157964199999999</v>
-      </c>
-      <c r="G8">
-        <v>9.28986014</v>
-      </c>
-    </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9">
-        <v>1.3149323500000001</v>
-      </c>
-      <c r="G9">
-        <v>9.0627885100000007</v>
-      </c>
-    </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10">
-        <v>1.4127403599999999</v>
-      </c>
-      <c r="G10">
-        <v>8.9377293600000005</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11">
-        <v>1.3454976400000001</v>
-      </c>
-      <c r="G11">
-        <v>8.7863482699999995</v>
-      </c>
-    </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12">
-        <v>1.2782549299999999</v>
-      </c>
-      <c r="G12">
-        <v>8.6349671800000003</v>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13">
-        <v>1.3088202200000001</v>
-      </c>
-      <c r="G13">
-        <v>8.3585269400000008</v>
-      </c>
-    </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.55000000000000004">
+        <v>21</v>
+      </c>
+      <c r="E13" s="10">
+        <v>5.2189553699999998</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1.4157964199999999</v>
+      </c>
+      <c r="G13" s="12">
+        <v>32.244994910000003</v>
+      </c>
+      <c r="H13" s="8">
+        <v>9.28986014</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14">
-        <v>1.2751988700000001</v>
-      </c>
-      <c r="G14">
-        <v>8.2828363899999999</v>
+        <v>5</v>
+      </c>
+      <c r="E14" s="10">
+        <v>5.2878471899999999</v>
+      </c>
+      <c r="F14" s="8">
+        <v>1.3149323500000001</v>
+      </c>
+      <c r="G14" s="12">
+        <v>31.903010590000001</v>
+      </c>
+      <c r="H14" s="8">
+        <v>9.0627885100000007</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="E15" s="10">
+        <v>4.9998104799999998</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1.4127403599999999</v>
+      </c>
+      <c r="G15" s="12">
+        <v>34.012756629999998</v>
+      </c>
+      <c r="H15" s="8">
+        <v>8.9377293600000005</v>
+      </c>
+      <c r="I15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="10">
+        <v>5.0457383599999996</v>
+      </c>
+      <c r="F16" s="8">
+        <v>1.3454976400000001</v>
+      </c>
+      <c r="G16" s="12">
+        <v>33.784767080000002</v>
+      </c>
+      <c r="H16" s="8">
+        <v>8.7863482699999995</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" ht="54" x14ac:dyDescent="0.55000000000000004">
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="10">
+        <v>5.0916662500000003</v>
+      </c>
+      <c r="F17" s="8">
+        <v>1.2782549299999999</v>
+      </c>
+      <c r="G17" s="12">
+        <v>33.556777529999998</v>
+      </c>
+      <c r="H17" s="8">
+        <v>8.6349671800000003</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" ht="54" x14ac:dyDescent="0.55000000000000004">
+      <c r="D18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="10">
+        <v>4.84955742</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1.3088202200000001</v>
+      </c>
+      <c r="G18" s="12">
+        <v>35.43853403</v>
+      </c>
+      <c r="H18" s="8">
+        <v>8.3585269400000008</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" ht="54" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="10">
+        <v>4.8725213600000004</v>
+      </c>
+      <c r="F19" s="8">
+        <v>1.2751988700000001</v>
+      </c>
+      <c r="G19" s="12">
+        <v>35.324539250000001</v>
+      </c>
+      <c r="H19" s="8">
+        <v>8.2828363899999999</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="4:10" ht="54" x14ac:dyDescent="0.55000000000000004">
+      <c r="D20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="11">
+        <v>4.8954852999999998</v>
+      </c>
+      <c r="F20" s="9">
         <v>1.2415775099999999</v>
       </c>
-      <c r="G15">
+      <c r="G20" s="13">
+        <v>35.210544480000003</v>
+      </c>
+      <c r="H20" s="9">
         <v>8.2071458400000008</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J20" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add chapter4folder and fix chapter3 folder name
</commit_message>
<xml_diff>
--- a/chapter2/input/chapter2_demo_data_prediction_result.xlsx
+++ b/chapter2/input/chapter2_demo_data_prediction_result.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\副業関連\独立\執筆\practical-mi-guide\chapter2\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295CB337-1ADE-413C-9991-363D6DBE72B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFB253D-7D27-472D-BD61-1377F90C010D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1310" yWindow="1290" windowWidth="30300" windowHeight="17850" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
+    <workbookView xWindow="6990" yWindow="1390" windowWidth="30300" windowHeight="17850" activeTab="1" xr2:uid="{AFFCA931-CB2A-4AED-B7E5-2638B5FCE6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="10" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
   <si>
     <t>画像濃度</t>
     <rPh sb="0" eb="4">
@@ -491,15 +492,44 @@
     <t>◎</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>ave</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>予測</t>
+    <rPh sb="0" eb="2">
+      <t>ヨソク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>実測</t>
+    <rPh sb="0" eb="2">
+      <t>ジッソク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>|予測―実測|</t>
+    <rPh sb="1" eb="4">
+      <t>ヨソクー</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ジッソク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.0"/>
+    <numFmt numFmtId="187" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -516,6 +546,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="游ゴシック"/>
@@ -657,7 +696,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -702,6 +741,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="187" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,8 +1249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3433FF01-647B-4F50-A819-EDB9541AAB09}">
   <dimension ref="D2:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView showGridLines="0" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1525,4 +1591,593 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A11B813-3861-4F6E-B524-82EDFB9C6B7E}">
+  <dimension ref="B1:N19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="2" max="2" width="18.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="10.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.74</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.13</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.04</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.53</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.09</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.84</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.64</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.45</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.59</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="10">
+        <v>5.1500635499999996</v>
+      </c>
+      <c r="D10" s="8">
+        <v>1.51666049</v>
+      </c>
+      <c r="E10" s="8">
+        <v>9.5169317800000002</v>
+      </c>
+      <c r="F10" s="8">
+        <v>32.586979229999997</v>
+      </c>
+      <c r="G10" s="15">
+        <v>5</v>
+      </c>
+      <c r="H10" s="16">
+        <v>1.64</v>
+      </c>
+      <c r="I10" s="15">
+        <v>10.3</v>
+      </c>
+      <c r="J10" s="17">
+        <v>32</v>
+      </c>
+      <c r="K10" s="23">
+        <f>ABS(C10-G10)</f>
+        <v>0.1500635499999996</v>
+      </c>
+      <c r="L10" s="23">
+        <f t="shared" ref="L10:N10" si="0">ABS(D10-H10)</f>
+        <v>0.12333950999999987</v>
+      </c>
+      <c r="M10" s="23">
+        <f t="shared" si="0"/>
+        <v>0.78306822000000054</v>
+      </c>
+      <c r="N10" s="23">
+        <f t="shared" si="0"/>
+        <v>0.58697922999999719</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="10">
+        <v>5.2189553699999998</v>
+      </c>
+      <c r="D11" s="8">
+        <v>1.4157964199999999</v>
+      </c>
+      <c r="E11" s="8">
+        <v>9.28986014</v>
+      </c>
+      <c r="F11" s="8">
+        <v>32.244994910000003</v>
+      </c>
+      <c r="G11" s="15">
+        <v>5</v>
+      </c>
+      <c r="H11" s="16">
+        <v>1.61</v>
+      </c>
+      <c r="I11" s="15">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J11" s="17">
+        <v>32</v>
+      </c>
+      <c r="K11" s="23">
+        <f t="shared" ref="K11:K18" si="1">ABS(C11-G11)</f>
+        <v>0.21895536999999976</v>
+      </c>
+      <c r="L11" s="23">
+        <f t="shared" ref="L11:L18" si="2">ABS(D11-H11)</f>
+        <v>0.19420358000000015</v>
+      </c>
+      <c r="M11" s="23">
+        <f t="shared" ref="M11:M18" si="3">ABS(E11-I11)</f>
+        <v>0.91013985999999925</v>
+      </c>
+      <c r="N11" s="23">
+        <f t="shared" ref="N11:N18" si="4">ABS(F11-J11)</f>
+        <v>0.24499491000000262</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="10">
+        <v>5.2878471899999999</v>
+      </c>
+      <c r="D12" s="8">
+        <v>1.3149323500000001</v>
+      </c>
+      <c r="E12" s="8">
+        <v>9.0627885100000007</v>
+      </c>
+      <c r="F12" s="8">
+        <v>31.903010590000001</v>
+      </c>
+      <c r="G12" s="15">
+        <v>5</v>
+      </c>
+      <c r="H12" s="16">
+        <v>1.57</v>
+      </c>
+      <c r="I12" s="15">
+        <v>10</v>
+      </c>
+      <c r="J12" s="17">
+        <v>32</v>
+      </c>
+      <c r="K12" s="23">
+        <f t="shared" si="1"/>
+        <v>0.28784718999999992</v>
+      </c>
+      <c r="L12" s="23">
+        <f t="shared" si="2"/>
+        <v>0.25506764999999998</v>
+      </c>
+      <c r="M12" s="23">
+        <f t="shared" si="3"/>
+        <v>0.93721148999999926</v>
+      </c>
+      <c r="N12" s="23">
+        <f t="shared" si="4"/>
+        <v>9.6989409999999054E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="10">
+        <v>4.9998104799999998</v>
+      </c>
+      <c r="D13" s="8">
+        <v>1.4127403599999999</v>
+      </c>
+      <c r="E13" s="8">
+        <v>8.9377293600000005</v>
+      </c>
+      <c r="F13" s="8">
+        <v>34.012756629999998</v>
+      </c>
+      <c r="G13" s="18">
+        <v>5</v>
+      </c>
+      <c r="H13" s="19">
+        <v>1.46</v>
+      </c>
+      <c r="I13" s="18">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J13" s="20">
+        <v>34</v>
+      </c>
+      <c r="K13" s="23">
+        <f t="shared" si="1"/>
+        <v>1.8952000000016511E-4</v>
+      </c>
+      <c r="L13" s="23">
+        <f t="shared" si="2"/>
+        <v>4.7259640000000047E-2</v>
+      </c>
+      <c r="M13" s="23">
+        <f t="shared" si="3"/>
+        <v>0.26227063999999878</v>
+      </c>
+      <c r="N13" s="23">
+        <f t="shared" si="4"/>
+        <v>1.2756629999998381E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10">
+        <v>5.0457383599999996</v>
+      </c>
+      <c r="D14" s="8">
+        <v>1.3454976400000001</v>
+      </c>
+      <c r="E14" s="8">
+        <v>8.7863482699999995</v>
+      </c>
+      <c r="F14" s="8">
+        <v>33.784767080000002</v>
+      </c>
+      <c r="G14" s="18">
+        <v>5</v>
+      </c>
+      <c r="H14" s="19">
+        <v>1.43</v>
+      </c>
+      <c r="I14" s="18">
+        <v>9.1</v>
+      </c>
+      <c r="J14" s="20">
+        <v>34</v>
+      </c>
+      <c r="K14" s="23">
+        <f t="shared" si="1"/>
+        <v>4.5738359999999645E-2</v>
+      </c>
+      <c r="L14" s="23">
+        <f t="shared" si="2"/>
+        <v>8.4502359999999888E-2</v>
+      </c>
+      <c r="M14" s="23">
+        <f t="shared" si="3"/>
+        <v>0.31365173000000013</v>
+      </c>
+      <c r="N14" s="23">
+        <f t="shared" si="4"/>
+        <v>0.21523291999999827</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="10">
+        <v>5.0916662500000003</v>
+      </c>
+      <c r="D15" s="8">
+        <v>1.2782549299999999</v>
+      </c>
+      <c r="E15" s="8">
+        <v>8.6349671800000003</v>
+      </c>
+      <c r="F15" s="8">
+        <v>33.556777529999998</v>
+      </c>
+      <c r="G15" s="18">
+        <v>5</v>
+      </c>
+      <c r="H15" s="19">
+        <v>1.41</v>
+      </c>
+      <c r="I15" s="18">
+        <v>9</v>
+      </c>
+      <c r="J15" s="20">
+        <v>34</v>
+      </c>
+      <c r="K15" s="23">
+        <f t="shared" si="1"/>
+        <v>9.1666250000000282E-2</v>
+      </c>
+      <c r="L15" s="23">
+        <f t="shared" si="2"/>
+        <v>0.13174507000000002</v>
+      </c>
+      <c r="M15" s="23">
+        <f t="shared" si="3"/>
+        <v>0.3650328199999997</v>
+      </c>
+      <c r="N15" s="23">
+        <f t="shared" si="4"/>
+        <v>0.44322247000000203</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B16" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="10">
+        <v>4.84955742</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1.3088202200000001</v>
+      </c>
+      <c r="E16" s="8">
+        <v>8.3585269400000008</v>
+      </c>
+      <c r="F16" s="8">
+        <v>35.43853403</v>
+      </c>
+      <c r="G16" s="15">
+        <v>5</v>
+      </c>
+      <c r="H16" s="16">
+        <v>1.25</v>
+      </c>
+      <c r="I16" s="15">
+        <v>8.1</v>
+      </c>
+      <c r="J16" s="17">
+        <v>35</v>
+      </c>
+      <c r="K16" s="23">
+        <f t="shared" si="1"/>
+        <v>0.15044257999999999</v>
+      </c>
+      <c r="L16" s="23">
+        <f t="shared" si="2"/>
+        <v>5.882022000000009E-2</v>
+      </c>
+      <c r="M16" s="23">
+        <f t="shared" si="3"/>
+        <v>0.2585269400000012</v>
+      </c>
+      <c r="N16" s="23">
+        <f t="shared" si="4"/>
+        <v>0.43853402999999958</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="10">
+        <v>4.8725213600000004</v>
+      </c>
+      <c r="D17" s="8">
+        <v>1.2751988700000001</v>
+      </c>
+      <c r="E17" s="8">
+        <v>8.2828363899999999</v>
+      </c>
+      <c r="F17" s="8">
+        <v>35.324539250000001</v>
+      </c>
+      <c r="G17" s="15">
+        <v>5</v>
+      </c>
+      <c r="H17" s="16">
+        <v>1.24</v>
+      </c>
+      <c r="I17" s="15">
+        <v>8.1</v>
+      </c>
+      <c r="J17" s="17">
+        <v>35</v>
+      </c>
+      <c r="K17" s="23">
+        <f t="shared" si="1"/>
+        <v>0.12747863999999964</v>
+      </c>
+      <c r="L17" s="23">
+        <f t="shared" si="2"/>
+        <v>3.5198870000000104E-2</v>
+      </c>
+      <c r="M17" s="23">
+        <f t="shared" si="3"/>
+        <v>0.18283639000000029</v>
+      </c>
+      <c r="N17" s="23">
+        <f t="shared" si="4"/>
+        <v>0.32453925000000083</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="10">
+        <v>4.8954852999999998</v>
+      </c>
+      <c r="D18" s="8">
+        <v>1.2415775099999999</v>
+      </c>
+      <c r="E18" s="8">
+        <v>8.2071458400000008</v>
+      </c>
+      <c r="F18" s="8">
+        <v>35.210544480000003</v>
+      </c>
+      <c r="G18" s="15">
+        <v>5</v>
+      </c>
+      <c r="H18" s="16">
+        <v>1.22</v>
+      </c>
+      <c r="I18" s="15">
+        <v>8</v>
+      </c>
+      <c r="J18" s="17">
+        <v>35</v>
+      </c>
+      <c r="K18" s="23">
+        <f t="shared" si="1"/>
+        <v>0.10451470000000018</v>
+      </c>
+      <c r="L18" s="23">
+        <f t="shared" si="2"/>
+        <v>2.1577509999999966E-2</v>
+      </c>
+      <c r="M18" s="23">
+        <f t="shared" si="3"/>
+        <v>0.2071458400000008</v>
+      </c>
+      <c r="N18" s="23">
+        <f t="shared" si="4"/>
+        <v>0.21054448000000292</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" s="21">
+        <f>AVERAGE((K10:K18))</f>
+        <v>0.13076623999999992</v>
+      </c>
+      <c r="L19" s="21">
+        <f t="shared" ref="L19:N19" si="5">AVERAGE((L10:L18))</f>
+        <v>0.10574604555555557</v>
+      </c>
+      <c r="M19" s="21">
+        <f t="shared" si="5"/>
+        <v>0.4688759922222222</v>
+      </c>
+      <c r="N19" s="21">
+        <f t="shared" si="5"/>
+        <v>0.28597703666666674</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>